<commit_message>
read and write xlsx files
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,123 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10368A45-05EB-48BD-8312-60C677F4EA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook" filterPrivacy="true"/>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>jwhite@domain.com</t>
-  </si>
-  <si>
-    <t>Borden</t>
-  </si>
-  <si>
-    <t>aborden@domain.com</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>mgreen@domain.com</t>
-  </si>
-  <si>
-    <t>Munsch</t>
-  </si>
-  <si>
-    <t>jmunsch@domain.com</t>
-  </si>
-  <si>
-    <t>Aragon</t>
-  </si>
-  <si>
-    <t>raragon@domain.com</t>
-  </si>
-  <si>
-    <t>Russell</t>
-  </si>
-  <si>
-    <t>jrussell@domain.com</t>
-  </si>
-  <si>
-    <t>Venson</t>
-  </si>
-  <si>
-    <t>lvenson@domain.com</t>
-  </si>
-  <si>
-    <t>Conley</t>
-  </si>
-  <si>
-    <t>tconley@domain.com</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>cjackson@domain.com</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>sdavis@domain.com</t>
-  </si>
-  <si>
-    <t>Watson</t>
-  </si>
-  <si>
-    <t>gwatson@domain.com</t>
-  </si>
-  <si>
-    <t>Garrison</t>
-  </si>
-  <si>
-    <t>lgarrison@domain.com</t>
-  </si>
-  <si>
-    <t>Renfro</t>
-  </si>
-  <si>
-    <t>jrenfro@domain.com</t>
-  </si>
-  <si>
-    <t>Heard</t>
-  </si>
-  <si>
-    <t>jheard@domain.com</t>
-  </si>
-  <si>
-    <t>Reyes</t>
-  </si>
-  <si>
-    <t>dreyes@domain.com</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -486,147 +396,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>email</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>White</v>
+      </c>
+      <c r="B2" t="str">
+        <v>jwhite@domain.com</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Borden</v>
+      </c>
+      <c r="B3" t="str">
+        <v>aborden@domain.com</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Green</v>
+      </c>
+      <c r="B4" t="str">
+        <v>mgreen@domain.com</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Munsch</v>
+      </c>
+      <c r="B5" t="str">
+        <v>jmunsch@domain.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Aragon</v>
+      </c>
+      <c r="B6" t="str">
+        <v>raragon@domain.com</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Russell</v>
+      </c>
+      <c r="B7" t="str">
+        <v>jrussell@domain.com</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Venson</v>
+      </c>
+      <c r="B8" t="str">
+        <v>lvenson@domain.com</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Conley</v>
+      </c>
+      <c r="B9" t="str">
+        <v>tconley@domain.com</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Jackson</v>
+      </c>
+      <c r="B10" t="str">
+        <v>cjackson@domain.com</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Davis</v>
+      </c>
+      <c r="B11" t="str">
+        <v>sdavis@domain.com</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Watson</v>
+      </c>
+      <c r="B12" t="str">
+        <v>gwatson@domain.com</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Garrison</v>
+      </c>
+      <c r="B13" t="str">
+        <v>lgarrison@domain.com</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Renfro</v>
+      </c>
+      <c r="B14" t="str">
+        <v>jrenfro@domain.com</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Heard</v>
+      </c>
+      <c r="B15" t="str">
+        <v>jheard@domain.com</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Reyes</v>
+      </c>
+      <c r="B16" t="str">
+        <v>dreyes@domain.com</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>qw</v>
+      </c>
+      <c r="B17" t="str">
+        <v>qw</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B16" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Electron app structure with xlsx file handling and UI enhancements
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
@@ -538,10 +538,18 @@
         <v>qw</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>rign</v>
+      </c>
+      <c r="B18" t="str">
+        <v>rimg@raidio.com</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>